<commit_message>
Bunch of doc updates to drop spurious index entries. Added a module name analysis to expl3-datatype-analysis.xlsx
</commit_message>
<xml_diff>
--- a/l3kernel/expl3-datatype-analysis.xlsx
+++ b/l3kernel/expl3-datatype-analysis.xlsx
@@ -4,16 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="21135" windowHeight="15225"/>
+    <workbookView xWindow="120" yWindow="255" windowWidth="21135" windowHeight="15225" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="data types" sheetId="1" r:id="rId1"/>
     <sheet name="constants" sheetId="4" r:id="rId2"/>
     <sheet name="oddities" sheetId="2" r:id="rId3"/>
+    <sheet name="Modules" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">constants!$A$1:$C$65</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'data types'!$A$2:$AT$327</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Modules!$A$1:$I$119</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -359,7 +361,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2716" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3110" uniqueCount="653">
   <si>
     <t>action</t>
   </si>
@@ -2027,6 +2029,300 @@
   </si>
   <si>
     <t>from_oct</t>
+  </si>
+  <si>
+    <t>Module name</t>
+  </si>
+  <si>
+    <t>chk</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Datatype</t>
+  </si>
+  <si>
+    <t>choice</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t>Keys</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>driver</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>these are actually all variables (where the data type is  at the end)</t>
+  </si>
+  <si>
+    <t>etex</t>
+  </si>
+  <si>
+    <t>primitives</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>flow/processing</t>
+  </si>
+  <si>
+    <t>fi</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>another example … foo?</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>hcoffins</t>
+  </si>
+  <si>
+    <t>initial</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>kernel</t>
+  </si>
+  <si>
+    <t>keys</t>
+  </si>
+  <si>
+    <t>what kind of thing is this? Datatype? (no "new")</t>
+  </si>
+  <si>
+    <t>keyval</t>
+  </si>
+  <si>
+    <t>LaTeX3 error</t>
+  </si>
+  <si>
+    <t>fake for expandable errors</t>
+  </si>
+  <si>
+    <t>lua</t>
+  </si>
+  <si>
+    <t>luatex</t>
+  </si>
+  <si>
+    <t>mark</t>
+  </si>
+  <si>
+    <t>quark only</t>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>minus</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>only exists as mode_if_...</t>
+  </si>
+  <si>
+    <t>msg</t>
+  </si>
+  <si>
+    <t>multichoice</t>
+  </si>
+  <si>
+    <t>multichoices</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>mymodule</t>
+  </si>
+  <si>
+    <t>mypkg</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>no_value</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>pdftex</t>
+  </si>
+  <si>
+    <t>pdttex</t>
+  </si>
+  <si>
+    <t>BUG :-)</t>
+  </si>
+  <si>
+    <t>prg</t>
+  </si>
+  <si>
+    <t>ptex</t>
+  </si>
+  <si>
+    <t>recursion_stop</t>
+  </si>
+  <si>
+    <t>reverse_if</t>
+  </si>
+  <si>
+    <t>recursion_tail</t>
+  </si>
+  <si>
+    <t>scan</t>
+  </si>
+  <si>
+    <t>spac</t>
+  </si>
+  <si>
+    <t>BUG ??? But even as space_... Questionable</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>quark and scan mark</t>
+  </si>
+  <si>
+    <t>kind of an input stream data type (no new or set etc operations)</t>
+  </si>
+  <si>
+    <t>tex</t>
+  </si>
+  <si>
+    <t>thirty</t>
+  </si>
+  <si>
+    <t>tmpa</t>
+  </si>
+  <si>
+    <t>tmpb</t>
+  </si>
+  <si>
+    <t>unicode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">these are actually all variables/constants (where the data type is  at the end)
+however, this may need to be a module one day (?) </t>
+  </si>
+  <si>
+    <t>uptex</t>
+  </si>
+  <si>
+    <t>utex</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>void</t>
+  </si>
+  <si>
+    <t>xetex</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Did we really needed both "lua" and "luatex"? Guess there are arguments either way</t>
+  </si>
+  <si>
+    <t>this sticks out a bit (in comparison to if_, say)</t>
+  </si>
+  <si>
+    <t>not a real module, should have perhaps been prg_... But too late to change</t>
+  </si>
+  <si>
+    <t>covers scan marks besides other things
+would also fall under the prg module really …</t>
+  </si>
+  <si>
+    <t>again really "prg_peek" but the commands are too long already</t>
+  </si>
+  <si>
+    <t>not a really module either but on the other hand not all of this would have been prg</t>
+  </si>
+  <si>
+    <t>!!</t>
+  </si>
+  <si>
+    <t>just some arbitrary example (should not show up in index and probably should not use "add") -- "foo" maybe?</t>
+  </si>
+  <si>
+    <t>should perhaps be _int to be consistent with variable/constant use in other types</t>
+  </si>
+  <si>
+    <t>need to think if h/vcoffins (as well as h/vbox) are really the right way to model this space</t>
+  </si>
+  <si>
+    <t>a bunch of them are used quite often (while :D commands!) so perhaps we need to have a closer look and either add interfaces or drop the usage</t>
+  </si>
+  <si>
+    <t>fully internal</t>
+  </si>
+  <si>
+    <t>questionable as a module; or if it is perhaps should get additional color handling commands (?)</t>
+  </si>
+  <si>
+    <t>fully internal (has only __kernel..) and only a few commands ; questionable</t>
+  </si>
+  <si>
+    <t>is that a data type or a flow control or what?</t>
+  </si>
+  <si>
+    <t>\show_until_if:w only in an example --- so drop and replace by something valid or at least make it not appear in the index</t>
+  </si>
+  <si>
+    <t>:-) but perhaps we want to always use "mymodule" as module name or maybe we always want to use foo but then consistently in all examples</t>
+  </si>
+  <si>
+    <t>nearly only internal and only one external command \keyval_parse:NNn. Strictly speaking this is really just \clist_keyval_parse:NNn with a clist in which = have additional meaning.
+My suggestion would be to drop that module and use \clist_keyval_parse:NNn or perhaps if prefered \keys_value_parse:NNn if you want to keep it with the keys module.</t>
+  </si>
+  <si>
+    <t>hide</t>
+  </si>
+  <si>
+    <t>these are actually all constants (where the data type is  at the end)</t>
   </si>
 </sst>
 </file>
@@ -2127,7 +2423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2274,6 +2570,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2581,8 +2883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AT333"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B275" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AH240" sqref="AH240"/>
@@ -2881,7 +3183,7 @@
       </c>
       <c r="AT3"/>
     </row>
-    <row r="4" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>96</v>
       </c>
@@ -2949,7 +3251,7 @@
       <c r="AS4" s="17"/>
       <c r="AT4"/>
     </row>
-    <row r="5" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>98</v>
       </c>
@@ -3015,7 +3317,7 @@
       <c r="AS5" s="17"/>
       <c r="AT5"/>
     </row>
-    <row r="6" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>147</v>
       </c>
@@ -3072,7 +3374,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>49</v>
       </c>
@@ -3147,7 +3449,7 @@
       </c>
       <c r="AS7" s="17"/>
     </row>
-    <row r="8" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>1</v>
       </c>
@@ -3243,7 +3545,7 @@
       </c>
       <c r="AS8" s="17"/>
     </row>
-    <row r="9" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>1</v>
       </c>
@@ -3288,7 +3590,7 @@
       </c>
       <c r="AS9" s="17"/>
     </row>
-    <row r="10" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>211</v>
       </c>
@@ -3333,7 +3635,7 @@
       </c>
       <c r="AS10" s="17"/>
     </row>
-    <row r="11" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>208</v>
       </c>
@@ -3378,7 +3680,7 @@
       </c>
       <c r="AS11" s="17"/>
     </row>
-    <row r="12" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>209</v>
       </c>
@@ -3423,7 +3725,7 @@
       </c>
       <c r="AS12" s="17"/>
     </row>
-    <row r="13" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>210</v>
       </c>
@@ -3468,7 +3770,7 @@
       </c>
       <c r="AS13" s="17"/>
     </row>
-    <row r="14" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
         <v>5</v>
       </c>
@@ -3558,7 +3860,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="15" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
         <v>5</v>
       </c>
@@ -3603,7 +3905,7 @@
       </c>
       <c r="AS15" s="33"/>
     </row>
-    <row r="16" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>5</v>
       </c>
@@ -3655,7 +3957,7 @@
       </c>
       <c r="AS16" s="17"/>
     </row>
-    <row r="17" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
         <v>5</v>
       </c>
@@ -3700,7 +4002,7 @@
       </c>
       <c r="AS17" s="34"/>
     </row>
-    <row r="18" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>507</v>
       </c>
@@ -3751,7 +4053,7 @@
       </c>
       <c r="AS18" s="33"/>
     </row>
-    <row r="19" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
         <v>5</v>
       </c>
@@ -3796,7 +4098,7 @@
       </c>
       <c r="AS19" s="17"/>
     </row>
-    <row r="20" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
         <v>14</v>
       </c>
@@ -3883,7 +4185,7 @@
       </c>
       <c r="AS20" s="17"/>
     </row>
-    <row r="21" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
         <v>403</v>
       </c>
@@ -3928,7 +4230,7 @@
       </c>
       <c r="AS21" s="33"/>
     </row>
-    <row r="22" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
         <v>404</v>
       </c>
@@ -3976,7 +4278,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="23" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
         <v>183</v>
       </c>
@@ -4021,7 +4323,7 @@
       </c>
       <c r="AS23" s="17"/>
     </row>
-    <row r="24" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>408</v>
       </c>
@@ -4066,7 +4368,7 @@
       </c>
       <c r="AS24" s="33"/>
     </row>
-    <row r="25" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
         <v>409</v>
       </c>
@@ -4111,7 +4413,7 @@
       </c>
       <c r="AS25" s="33"/>
     </row>
-    <row r="26" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A26" s="36" t="s">
         <v>410</v>
       </c>
@@ -4156,7 +4458,7 @@
       </c>
       <c r="AS26" s="33"/>
     </row>
-    <row r="27" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A27" s="36" t="s">
         <v>411</v>
       </c>
@@ -4201,7 +4503,7 @@
       </c>
       <c r="AS27" s="33"/>
     </row>
-    <row r="28" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
         <v>412</v>
       </c>
@@ -4246,7 +4548,7 @@
       </c>
       <c r="AS28" s="33"/>
     </row>
-    <row r="29" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
         <v>413</v>
       </c>
@@ -4291,7 +4593,7 @@
       </c>
       <c r="AS29" s="33"/>
     </row>
-    <row r="30" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A30" s="36" t="s">
         <v>414</v>
       </c>
@@ -4336,7 +4638,7 @@
       </c>
       <c r="AS30" s="33"/>
     </row>
-    <row r="31" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
         <v>415</v>
       </c>
@@ -4381,7 +4683,7 @@
       </c>
       <c r="AS31" s="33"/>
     </row>
-    <row r="32" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
         <v>416</v>
       </c>
@@ -4426,7 +4728,7 @@
       </c>
       <c r="AS32" s="33"/>
     </row>
-    <row r="33" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
         <v>417</v>
       </c>
@@ -4471,7 +4773,7 @@
       </c>
       <c r="AS33" s="33"/>
     </row>
-    <row r="34" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
         <v>418</v>
       </c>
@@ -4516,7 +4818,7 @@
       </c>
       <c r="AS34" s="33"/>
     </row>
-    <row r="35" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
         <v>419</v>
       </c>
@@ -4561,7 +4863,7 @@
       </c>
       <c r="AS35" s="33"/>
     </row>
-    <row r="36" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
         <v>420</v>
       </c>
@@ -4606,7 +4908,7 @@
       </c>
       <c r="AS36" s="33"/>
     </row>
-    <row r="37" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A37" s="36" t="s">
         <v>421</v>
       </c>
@@ -4651,7 +4953,7 @@
       </c>
       <c r="AS37" s="33"/>
     </row>
-    <row r="38" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A38" s="36" t="s">
         <v>422</v>
       </c>
@@ -4696,7 +4998,7 @@
       </c>
       <c r="AS38" s="33"/>
     </row>
-    <row r="39" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A39" s="36" t="s">
         <v>423</v>
       </c>
@@ -4741,7 +5043,7 @@
       </c>
       <c r="AS39" s="33"/>
     </row>
-    <row r="40" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A40" s="36" t="s">
         <v>406</v>
       </c>
@@ -4786,7 +5088,7 @@
       </c>
       <c r="AS40" s="33"/>
     </row>
-    <row r="41" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="36" t="s">
         <v>7</v>
       </c>
@@ -4834,7 +5136,7 @@
       </c>
       <c r="AS41" s="17"/>
     </row>
-    <row r="42" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="36" t="s">
         <v>465</v>
       </c>
@@ -4879,7 +5181,7 @@
       </c>
       <c r="AS42" s="33"/>
     </row>
-    <row r="43" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="36" t="s">
         <v>165</v>
       </c>
@@ -4927,7 +5229,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="44" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="36" t="s">
         <v>165</v>
       </c>
@@ -4975,7 +5277,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="45" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="36" t="s">
         <v>214</v>
       </c>
@@ -5020,7 +5322,7 @@
       </c>
       <c r="AS45" s="17"/>
     </row>
-    <row r="46" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="36" t="s">
         <v>172</v>
       </c>
@@ -5065,7 +5367,7 @@
       </c>
       <c r="AS46" s="33"/>
     </row>
-    <row r="47" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="36" t="s">
         <v>425</v>
       </c>
@@ -5111,7 +5413,7 @@
       </c>
       <c r="AS47" s="33"/>
     </row>
-    <row r="48" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="36" t="s">
         <v>467</v>
       </c>
@@ -5156,7 +5458,7 @@
       </c>
       <c r="AS48" s="33"/>
     </row>
-    <row r="49" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="36" t="s">
         <v>426</v>
       </c>
@@ -5202,7 +5504,7 @@
       </c>
       <c r="AS49" s="17"/>
     </row>
-    <row r="50" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
         <v>203</v>
       </c>
@@ -5247,7 +5549,7 @@
       </c>
       <c r="AS50" s="17"/>
     </row>
-    <row r="51" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="36" t="s">
         <v>204</v>
       </c>
@@ -5292,7 +5594,7 @@
       </c>
       <c r="AS51" s="17"/>
     </row>
-    <row r="52" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:46" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="36" t="s">
         <v>205</v>
       </c>
@@ -5337,7 +5639,7 @@
       </c>
       <c r="AS52" s="17"/>
     </row>
-    <row r="53" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="36" t="s">
         <v>111</v>
       </c>
@@ -5382,7 +5684,7 @@
       </c>
       <c r="AS53" s="17"/>
     </row>
-    <row r="54" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="36" t="s">
         <v>427</v>
       </c>
@@ -5428,7 +5730,7 @@
       </c>
       <c r="AS54" s="33"/>
     </row>
-    <row r="55" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="36" t="s">
         <v>167</v>
       </c>
@@ -5476,7 +5778,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="56" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="36" t="s">
         <v>510</v>
       </c>
@@ -5521,7 +5823,7 @@
       </c>
       <c r="AS56" s="34"/>
     </row>
-    <row r="57" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="36" t="s">
         <v>508</v>
       </c>
@@ -5566,7 +5868,7 @@
       </c>
       <c r="AS57" s="34"/>
     </row>
-    <row r="58" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="36" t="s">
         <v>520</v>
       </c>
@@ -5614,7 +5916,7 @@
       </c>
       <c r="AS58" s="34"/>
     </row>
-    <row r="59" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="36" t="s">
         <v>512</v>
       </c>
@@ -5659,7 +5961,7 @@
       </c>
       <c r="AS59" s="34"/>
     </row>
-    <row r="60" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="36" t="s">
         <v>8</v>
       </c>
@@ -5707,7 +6009,7 @@
       </c>
       <c r="AS60" s="17"/>
     </row>
-    <row r="61" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="36" t="s">
         <v>428</v>
       </c>
@@ -5753,7 +6055,7 @@
       </c>
       <c r="AS61" s="17"/>
     </row>
-    <row r="62" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="36" t="s">
         <v>212</v>
       </c>
@@ -5795,7 +6097,7 @@
       </c>
       <c r="AS62" s="17"/>
     </row>
-    <row r="63" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="36" t="s">
         <v>51</v>
       </c>
@@ -5855,7 +6157,7 @@
       </c>
       <c r="AS63" s="27"/>
     </row>
-    <row r="64" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="36" t="s">
         <v>289</v>
       </c>
@@ -5915,7 +6217,7 @@
       </c>
       <c r="AS64" s="17"/>
     </row>
-    <row r="65" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:46" s="1" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="43" t="str">
         <f t="shared" si="1"/>
@@ -6093,7 +6395,7 @@
       </c>
       <c r="AT66"/>
     </row>
-    <row r="67" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="36" t="s">
         <v>493</v>
       </c>
@@ -6141,7 +6443,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="68" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="36" t="s">
         <v>159</v>
       </c>
@@ -6189,7 +6491,7 @@
       </c>
       <c r="AS68" s="17"/>
     </row>
-    <row r="69" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="36" t="s">
         <v>175</v>
       </c>
@@ -6234,7 +6536,7 @@
       </c>
       <c r="AS69" s="17"/>
     </row>
-    <row r="70" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="36" t="s">
         <v>177</v>
       </c>
@@ -6282,7 +6584,7 @@
       </c>
       <c r="AS70" s="17"/>
     </row>
-    <row r="71" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="36" t="s">
         <v>99</v>
       </c>
@@ -6336,7 +6638,7 @@
       </c>
       <c r="AS71" s="17"/>
     </row>
-    <row r="72" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="36" t="s">
         <v>101</v>
       </c>
@@ -6390,7 +6692,7 @@
       </c>
       <c r="AS72" s="17"/>
     </row>
-    <row r="73" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:46" s="1" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="43" t="str">
         <f t="shared" si="1"/>
@@ -6578,7 +6880,7 @@
       </c>
       <c r="AT74"/>
     </row>
-    <row r="75" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="36" t="s">
         <v>158</v>
       </c>
@@ -6630,7 +6932,7 @@
       <c r="AS75" s="17"/>
       <c r="AT75"/>
     </row>
-    <row r="76" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="36" t="s">
         <v>158</v>
       </c>
@@ -6678,7 +6980,7 @@
       </c>
       <c r="AS76" s="17"/>
     </row>
-    <row r="77" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="36" t="s">
         <v>154</v>
       </c>
@@ -6726,7 +7028,7 @@
       </c>
       <c r="AS77" s="17"/>
     </row>
-    <row r="78" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="36" t="s">
         <v>155</v>
       </c>
@@ -6774,7 +7076,7 @@
       </c>
       <c r="AS78" s="17"/>
     </row>
-    <row r="79" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="36" t="s">
         <v>494</v>
       </c>
@@ -6819,7 +7121,7 @@
       </c>
       <c r="AS79" s="33"/>
     </row>
-    <row r="80" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="36" t="s">
         <v>286</v>
       </c>
@@ -6868,7 +7170,7 @@
       <c r="AS80" s="17"/>
       <c r="AT80" s="10"/>
     </row>
-    <row r="81" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="36" t="s">
         <v>109</v>
       </c>
@@ -6920,7 +7222,7 @@
       <c r="AS81" s="17"/>
       <c r="AT81" s="10"/>
     </row>
-    <row r="82" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="36" t="s">
         <v>157</v>
       </c>
@@ -6968,7 +7270,7 @@
       </c>
       <c r="AS82" s="17"/>
     </row>
-    <row r="83" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="36" t="s">
         <v>108</v>
       </c>
@@ -7019,7 +7321,7 @@
       </c>
       <c r="AS83" s="17"/>
     </row>
-    <row r="84" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:46" s="1" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="43" t="str">
         <f t="shared" si="21"/>
@@ -7207,7 +7509,7 @@
       </c>
       <c r="AT85"/>
     </row>
-    <row r="86" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="36" t="s">
         <v>488</v>
       </c>
@@ -7256,7 +7558,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="87" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="36" t="s">
         <v>6</v>
       </c>
@@ -7313,7 +7615,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="88" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="36" t="s">
         <v>6</v>
       </c>
@@ -7362,7 +7664,7 @@
       <c r="AS88" s="17"/>
       <c r="AT88"/>
     </row>
-    <row r="89" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="38" t="s">
         <v>291</v>
       </c>
@@ -7419,7 +7721,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="90" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="36" t="s">
         <v>151</v>
       </c>
@@ -7467,7 +7769,7 @@
       </c>
       <c r="AS90" s="17"/>
     </row>
-    <row r="91" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="36" t="s">
         <v>152</v>
       </c>
@@ -7515,7 +7817,7 @@
       </c>
       <c r="AS91" s="17"/>
     </row>
-    <row r="92" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="36" t="s">
         <v>135</v>
       </c>
@@ -7566,7 +7868,7 @@
       </c>
       <c r="AS92" s="17"/>
     </row>
-    <row r="93" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="36" t="s">
         <v>532</v>
       </c>
@@ -7614,7 +7916,7 @@
       </c>
       <c r="AS93" s="44"/>
     </row>
-    <row r="94" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="36" t="s">
         <v>135</v>
       </c>
@@ -7665,7 +7967,7 @@
       </c>
       <c r="AS94" s="17"/>
     </row>
-    <row r="95" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="36" t="s">
         <v>161</v>
       </c>
@@ -7719,7 +8021,7 @@
       </c>
       <c r="AS95" s="25"/>
     </row>
-    <row r="96" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="36" t="s">
         <v>161</v>
       </c>
@@ -7767,7 +8069,7 @@
       </c>
       <c r="AS96" s="52"/>
     </row>
-    <row r="97" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="36" t="s">
         <v>161</v>
       </c>
@@ -7820,7 +8122,7 @@
       <c r="AS97" s="17"/>
       <c r="AT97" s="10"/>
     </row>
-    <row r="98" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="36" t="s">
         <v>534</v>
       </c>
@@ -7854,7 +8156,7 @@
       <c r="AS98" s="44"/>
       <c r="AT98" s="10"/>
     </row>
-    <row r="99" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" s="36" t="s">
         <v>534</v>
       </c>
@@ -7888,7 +8190,7 @@
       <c r="AS99" s="44"/>
       <c r="AT99" s="10"/>
     </row>
-    <row r="100" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="36" t="s">
         <v>537</v>
       </c>
@@ -7922,7 +8224,7 @@
       <c r="AS100" s="44"/>
       <c r="AT100" s="10"/>
     </row>
-    <row r="101" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="36" t="s">
         <v>136</v>
       </c>
@@ -7970,7 +8272,7 @@
       </c>
       <c r="AS101" s="25"/>
     </row>
-    <row r="102" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" s="36" t="s">
         <v>533</v>
       </c>
@@ -8015,7 +8317,7 @@
       </c>
       <c r="AS102" s="44"/>
     </row>
-    <row r="103" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="36" t="s">
         <v>136</v>
       </c>
@@ -8063,7 +8365,7 @@
       </c>
       <c r="AS103" s="17"/>
     </row>
-    <row r="104" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:46" s="1" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="B104" s="43" t="str">
         <f t="shared" si="21"/>
@@ -8251,7 +8553,7 @@
       </c>
       <c r="AT105"/>
     </row>
-    <row r="106" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A106" s="36" t="s">
         <v>54</v>
       </c>
@@ -8309,7 +8611,7 @@
       <c r="AS106" s="17"/>
       <c r="AT106"/>
     </row>
-    <row r="107" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="36" t="s">
         <v>240</v>
       </c>
@@ -8354,7 +8656,7 @@
       </c>
       <c r="AS107" s="17"/>
     </row>
-    <row r="108" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="36" t="s">
         <v>395</v>
       </c>
@@ -8397,7 +8699,7 @@
       <c r="AS108" s="17"/>
       <c r="AT108"/>
     </row>
-    <row r="109" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="36" t="s">
         <v>55</v>
       </c>
@@ -8443,7 +8745,7 @@
       <c r="AS109" s="17"/>
       <c r="AT109"/>
     </row>
-    <row r="110" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A110" s="36" t="s">
         <v>56</v>
       </c>
@@ -8489,7 +8791,7 @@
       <c r="AS110" s="17"/>
       <c r="AT110"/>
     </row>
-    <row r="111" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A111" s="36" t="s">
         <v>241</v>
       </c>
@@ -8534,7 +8836,7 @@
       </c>
       <c r="AS111" s="17"/>
     </row>
-    <row r="112" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A112" s="36" t="s">
         <v>107</v>
       </c>
@@ -8579,7 +8881,7 @@
       </c>
       <c r="AS112" s="17"/>
     </row>
-    <row r="113" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A113" s="36" t="s">
         <v>102</v>
       </c>
@@ -8624,7 +8926,7 @@
       </c>
       <c r="AS113" s="17"/>
     </row>
-    <row r="114" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A114" s="36" t="s">
         <v>236</v>
       </c>
@@ -8669,7 +8971,7 @@
       </c>
       <c r="AS114" s="17"/>
     </row>
-    <row r="115" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A115" s="36" t="s">
         <v>398</v>
       </c>
@@ -8714,7 +9016,7 @@
       </c>
       <c r="AS115" s="33"/>
     </row>
-    <row r="116" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A116" s="36" t="s">
         <v>399</v>
       </c>
@@ -8759,7 +9061,7 @@
       </c>
       <c r="AS116" s="33"/>
     </row>
-    <row r="117" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A117" s="36" t="s">
         <v>133</v>
       </c>
@@ -8810,7 +9112,7 @@
       </c>
       <c r="AS117" s="17"/>
     </row>
-    <row r="118" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A118" s="36" t="s">
         <v>237</v>
       </c>
@@ -8855,7 +9157,7 @@
       </c>
       <c r="AS118" s="17"/>
     </row>
-    <row r="119" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A119" s="36" t="s">
         <v>238</v>
       </c>
@@ -8900,7 +9202,7 @@
       </c>
       <c r="AS119" s="33"/>
     </row>
-    <row r="120" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A120" s="36" t="s">
         <v>193</v>
       </c>
@@ -8948,7 +9250,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="121" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A121" s="36" t="s">
         <v>232</v>
       </c>
@@ -8990,7 +9292,7 @@
       </c>
       <c r="AS121" s="17"/>
     </row>
-    <row r="122" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A122" s="36" t="s">
         <v>194</v>
       </c>
@@ -9038,7 +9340,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="123" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A123" s="36" t="s">
         <v>233</v>
       </c>
@@ -9080,7 +9382,7 @@
       </c>
       <c r="AS123" s="17"/>
     </row>
-    <row r="124" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A124" s="36" t="s">
         <v>195</v>
       </c>
@@ -9128,7 +9430,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="125" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A125" s="36" t="s">
         <v>60</v>
       </c>
@@ -9185,7 +9487,7 @@
       </c>
       <c r="AS125" s="29"/>
     </row>
-    <row r="126" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A126" s="36" t="s">
         <v>401</v>
       </c>
@@ -9233,7 +9535,7 @@
       </c>
       <c r="AS126" s="33"/>
     </row>
-    <row r="127" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A127" s="36" t="s">
         <v>134</v>
       </c>
@@ -9278,7 +9580,7 @@
       </c>
       <c r="AS127" s="33"/>
     </row>
-    <row r="128" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A128" s="36" t="s">
         <v>402</v>
       </c>
@@ -9326,7 +9628,7 @@
       </c>
       <c r="AS128" s="33"/>
     </row>
-    <row r="129" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:46" s="1" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="43" t="str">
         <f t="shared" si="21"/>
@@ -9513,7 +9815,7 @@
       </c>
       <c r="AT130"/>
     </row>
-    <row r="131" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A131" s="36" t="s">
         <v>284</v>
       </c>
@@ -9568,7 +9870,7 @@
       <c r="AS131" s="17"/>
       <c r="AT131"/>
     </row>
-    <row r="132" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A132" s="36" t="s">
         <v>284</v>
       </c>
@@ -9617,7 +9919,7 @@
       <c r="AS132" s="17"/>
       <c r="AT132"/>
     </row>
-    <row r="133" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A133" s="36" t="s">
         <v>530</v>
       </c>
@@ -9666,7 +9968,7 @@
       <c r="AS133" s="44"/>
       <c r="AT133"/>
     </row>
-    <row r="134" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A134" s="36" t="s">
         <v>531</v>
       </c>
@@ -9715,7 +10017,7 @@
       <c r="AS134" s="44"/>
       <c r="AT134"/>
     </row>
-    <row r="135" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A135" s="36" t="s">
         <v>531</v>
       </c>
@@ -9764,7 +10066,7 @@
       <c r="AS135" s="44"/>
       <c r="AT135"/>
     </row>
-    <row r="136" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A136" s="36" t="s">
         <v>285</v>
       </c>
@@ -9813,7 +10115,7 @@
       <c r="AS136" s="17"/>
       <c r="AT136"/>
     </row>
-    <row r="137" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A137" s="36" t="s">
         <v>190</v>
       </c>
@@ -9865,7 +10167,7 @@
       <c r="AS137" s="17"/>
       <c r="AT137"/>
     </row>
-    <row r="138" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A138" s="36" t="s">
         <v>192</v>
       </c>
@@ -9917,7 +10219,7 @@
       <c r="AS138" s="17"/>
       <c r="AT138"/>
     </row>
-    <row r="139" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A139" s="36" t="s">
         <v>207</v>
       </c>
@@ -9968,7 +10270,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="140" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A140" s="36" t="s">
         <v>191</v>
       </c>
@@ -10019,7 +10321,7 @@
       </c>
       <c r="AS140" s="17"/>
     </row>
-    <row r="141" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:46" s="1" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
       <c r="B141" s="43" t="str">
         <f t="shared" si="21"/>
@@ -10202,7 +10504,7 @@
       </c>
       <c r="AT142"/>
     </row>
-    <row r="143" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A143" s="36" t="s">
         <v>470</v>
       </c>
@@ -10250,7 +10552,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="144" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A144" s="36" t="s">
         <v>440</v>
       </c>
@@ -10307,7 +10609,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="145" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A145" s="36" t="s">
         <v>440</v>
       </c>
@@ -10358,7 +10660,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="146" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A146" s="36" t="s">
         <v>445</v>
       </c>
@@ -10406,7 +10708,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="147" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A147" s="36" t="s">
         <v>474</v>
       </c>
@@ -10452,7 +10754,7 @@
       <c r="AS147" s="33"/>
       <c r="AT147"/>
     </row>
-    <row r="148" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A148" s="36" t="s">
         <v>475</v>
       </c>
@@ -10500,7 +10802,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="149" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A149" s="36" t="s">
         <v>476</v>
       </c>
@@ -10548,7 +10850,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="150" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A150" s="36" t="s">
         <v>477</v>
       </c>
@@ -10596,7 +10898,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="151" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A151" s="36" t="s">
         <v>478</v>
       </c>
@@ -10644,7 +10946,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="152" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A152" s="36" t="s">
         <v>479</v>
       </c>
@@ -10692,7 +10994,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="153" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A153" s="36" t="s">
         <v>480</v>
       </c>
@@ -10740,7 +11042,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="154" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A154" s="36" t="s">
         <v>481</v>
       </c>
@@ -10788,7 +11090,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="155" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A155" s="36" t="s">
         <v>61</v>
       </c>
@@ -10840,7 +11142,7 @@
       <c r="AS155" s="33"/>
       <c r="AT155"/>
     </row>
-    <row r="156" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A156" s="36" t="s">
         <v>61</v>
       </c>
@@ -10892,7 +11194,7 @@
       <c r="AS156" s="33"/>
       <c r="AT156"/>
     </row>
-    <row r="157" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A157" s="36" t="s">
         <v>66</v>
       </c>
@@ -10944,7 +11246,7 @@
       <c r="AS157" s="33"/>
       <c r="AT157"/>
     </row>
-    <row r="158" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A158" s="36" t="s">
         <v>66</v>
       </c>
@@ -10999,7 +11301,7 @@
       <c r="AS158" s="33"/>
       <c r="AT158"/>
     </row>
-    <row r="159" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A159" s="36" t="s">
         <v>66</v>
       </c>
@@ -11048,7 +11350,7 @@
       <c r="AS159" s="33"/>
       <c r="AT159"/>
     </row>
-    <row r="160" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A160" s="36" t="s">
         <v>67</v>
       </c>
@@ -11100,7 +11402,7 @@
       <c r="AS160" s="33"/>
       <c r="AT160"/>
     </row>
-    <row r="161" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A161" s="36" t="s">
         <v>67</v>
       </c>
@@ -11155,7 +11457,7 @@
       <c r="AS161" s="17"/>
       <c r="AT161"/>
     </row>
-    <row r="162" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A162" s="36" t="s">
         <v>67</v>
       </c>
@@ -11203,7 +11505,7 @@
       </c>
       <c r="AS162" s="17"/>
     </row>
-    <row r="163" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A163" s="36" t="s">
         <v>22</v>
       </c>
@@ -11252,7 +11554,7 @@
       </c>
       <c r="AS163" s="17"/>
     </row>
-    <row r="164" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A164" s="36" t="s">
         <v>22</v>
       </c>
@@ -11298,7 +11600,7 @@
       </c>
       <c r="AS164" s="17"/>
     </row>
-    <row r="165" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A165" s="36" t="s">
         <v>117</v>
       </c>
@@ -11346,7 +11648,7 @@
       </c>
       <c r="AS165" s="17"/>
     </row>
-    <row r="166" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A166" s="36" t="s">
         <v>451</v>
       </c>
@@ -11394,7 +11696,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="167" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A167" s="36" t="s">
         <v>118</v>
       </c>
@@ -11457,7 +11759,7 @@
       </c>
       <c r="AS167" s="17"/>
     </row>
-    <row r="168" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A168" s="36" t="s">
         <v>118</v>
       </c>
@@ -11508,7 +11810,7 @@
       </c>
       <c r="AS168" s="17"/>
     </row>
-    <row r="169" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A169" s="36" t="s">
         <v>119</v>
       </c>
@@ -11556,7 +11858,7 @@
       </c>
       <c r="AS169" s="17"/>
     </row>
-    <row r="170" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A170" s="36" t="s">
         <v>119</v>
       </c>
@@ -11604,7 +11906,7 @@
       </c>
       <c r="AS170" s="33"/>
     </row>
-    <row r="171" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A171" s="36" t="s">
         <v>119</v>
       </c>
@@ -11652,7 +11954,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="172" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A172" s="36" t="s">
         <v>447</v>
       </c>
@@ -11697,7 +11999,7 @@
       </c>
       <c r="AS172" s="33"/>
     </row>
-    <row r="173" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A173" s="36" t="s">
         <v>448</v>
       </c>
@@ -11742,7 +12044,7 @@
       </c>
       <c r="AS173" s="33"/>
     </row>
-    <row r="174" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A174" s="36" t="s">
         <v>449</v>
       </c>
@@ -11787,7 +12089,7 @@
       </c>
       <c r="AS174" s="33"/>
     </row>
-    <row r="175" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A175" s="36" t="s">
         <v>314</v>
       </c>
@@ -11836,7 +12138,7 @@
       <c r="AS175" s="33"/>
       <c r="AT175" s="7"/>
     </row>
-    <row r="176" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A176" s="36" t="s">
         <v>64</v>
       </c>
@@ -11881,7 +12183,7 @@
       </c>
       <c r="AS176" s="33"/>
     </row>
-    <row r="177" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A177" s="36" t="s">
         <v>206</v>
       </c>
@@ -11973,7 +12275,7 @@
       </c>
       <c r="AS177" s="33"/>
     </row>
-    <row r="178" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A178" s="36" t="s">
         <v>206</v>
       </c>
@@ -12034,7 +12336,7 @@
       <c r="AO178" s="9"/>
       <c r="AS178" s="33"/>
     </row>
-    <row r="179" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A179" s="36" t="s">
         <v>462</v>
       </c>
@@ -12096,7 +12398,7 @@
       <c r="AO179" s="9"/>
       <c r="AS179" s="17"/>
     </row>
-    <row r="180" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A180" s="36" t="s">
         <v>278</v>
       </c>
@@ -12144,7 +12446,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="181" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A181" s="36" t="s">
         <v>434</v>
       </c>
@@ -12189,7 +12491,7 @@
       </c>
       <c r="AS181" s="17"/>
     </row>
-    <row r="182" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A182" s="36" t="s">
         <v>139</v>
       </c>
@@ -12234,7 +12536,7 @@
       </c>
       <c r="AS182" s="17"/>
     </row>
-    <row r="183" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A183" s="36" t="s">
         <v>138</v>
       </c>
@@ -12279,7 +12581,7 @@
       </c>
       <c r="AS183" s="33"/>
     </row>
-    <row r="184" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A184" s="36" t="s">
         <v>141</v>
       </c>
@@ -12324,7 +12626,7 @@
       </c>
       <c r="AS184" s="17"/>
     </row>
-    <row r="185" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A185" s="36" t="s">
         <v>318</v>
       </c>
@@ -12369,7 +12671,7 @@
       </c>
       <c r="AS185" s="33"/>
     </row>
-    <row r="186" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A186" s="36" t="s">
         <v>319</v>
       </c>
@@ -12414,7 +12716,7 @@
       </c>
       <c r="AS186" s="24"/>
     </row>
-    <row r="187" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A187" s="36" t="s">
         <v>320</v>
       </c>
@@ -12459,7 +12761,7 @@
       </c>
       <c r="AS187" s="17"/>
     </row>
-    <row r="188" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A188" s="36" t="s">
         <v>197</v>
       </c>
@@ -12507,7 +12809,7 @@
       </c>
       <c r="AS188" s="17"/>
     </row>
-    <row r="189" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" s="36" t="s">
         <v>121</v>
       </c>
@@ -12564,7 +12866,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="190" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A190" s="36" t="s">
         <v>121</v>
       </c>
@@ -12615,7 +12917,7 @@
       </c>
       <c r="AS190" s="17"/>
     </row>
-    <row r="191" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" s="36" t="s">
         <v>452</v>
       </c>
@@ -12663,7 +12965,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="192" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A192" s="36" t="s">
         <v>453</v>
       </c>
@@ -12711,7 +13013,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="193" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A193" s="36" t="s">
         <v>32</v>
       </c>
@@ -12759,7 +13061,7 @@
       </c>
       <c r="AS193" s="17"/>
     </row>
-    <row r="194" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A194" s="36" t="s">
         <v>33</v>
       </c>
@@ -12807,7 +13109,7 @@
       </c>
       <c r="AS194" s="17"/>
     </row>
-    <row r="195" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A195" s="36" t="s">
         <v>65</v>
       </c>
@@ -12852,7 +13154,7 @@
       </c>
       <c r="AS195" s="17"/>
     </row>
-    <row r="196" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A196" s="36" t="s">
         <v>122</v>
       </c>
@@ -12897,7 +13199,7 @@
       </c>
       <c r="AS196" s="17"/>
     </row>
-    <row r="197" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A197" s="36" t="s">
         <v>122</v>
       </c>
@@ -12942,7 +13244,7 @@
       </c>
       <c r="AS197" s="17"/>
     </row>
-    <row r="198" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A198" s="36" t="s">
         <v>123</v>
       </c>
@@ -12990,7 +13292,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="199" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A199" s="36" t="s">
         <v>454</v>
       </c>
@@ -13038,7 +13340,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="200" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A200" s="36" t="s">
         <v>455</v>
       </c>
@@ -13086,7 +13388,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="201" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A201" s="36" t="s">
         <v>198</v>
       </c>
@@ -13134,7 +13436,7 @@
       </c>
       <c r="AS201" s="17"/>
     </row>
-    <row r="202" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A202" s="36" t="s">
         <v>491</v>
       </c>
@@ -13182,7 +13484,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="203" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A203" s="36" t="s">
         <v>207</v>
       </c>
@@ -13230,7 +13532,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="204" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A204" s="36" t="s">
         <v>482</v>
       </c>
@@ -13278,7 +13580,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="205" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A205" s="36" t="s">
         <v>483</v>
       </c>
@@ -13326,7 +13628,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="206" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A206" s="36" t="s">
         <v>484</v>
       </c>
@@ -13374,7 +13676,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="207" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A207" s="36" t="s">
         <v>485</v>
       </c>
@@ -13417,7 +13719,7 @@
       <c r="AS207" s="33"/>
       <c r="AT207"/>
     </row>
-    <row r="208" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A208" s="36" t="s">
         <v>296</v>
       </c>
@@ -13462,7 +13764,7 @@
       </c>
       <c r="AS208" s="31"/>
     </row>
-    <row r="209" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" s="36" t="s">
         <v>294</v>
       </c>
@@ -13507,7 +13809,7 @@
       </c>
       <c r="AS209" s="31"/>
     </row>
-    <row r="210" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A210" s="36" t="s">
         <v>297</v>
       </c>
@@ -13552,7 +13854,7 @@
       </c>
       <c r="AS210" s="31"/>
     </row>
-    <row r="211" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A211" s="36" t="s">
         <v>25</v>
       </c>
@@ -13600,7 +13902,7 @@
       </c>
       <c r="AS211" s="17"/>
     </row>
-    <row r="212" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A212" s="36" t="s">
         <v>25</v>
       </c>
@@ -13651,7 +13953,7 @@
       </c>
       <c r="AS212" s="24"/>
     </row>
-    <row r="213" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A213" s="36" t="s">
         <v>25</v>
       </c>
@@ -13705,7 +14007,7 @@
       </c>
       <c r="AS213" s="17"/>
     </row>
-    <row r="214" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A214" s="36" t="s">
         <v>29</v>
       </c>
@@ -13753,7 +14055,7 @@
       </c>
       <c r="AS214" s="17"/>
     </row>
-    <row r="215" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A215" s="36" t="s">
         <v>29</v>
       </c>
@@ -13804,7 +14106,7 @@
       </c>
       <c r="AS215" s="17"/>
     </row>
-    <row r="216" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A216" s="36" t="s">
         <v>29</v>
       </c>
@@ -13858,7 +14160,7 @@
       </c>
       <c r="AS216" s="24"/>
     </row>
-    <row r="217" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:46" s="1" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A217" s="5"/>
       <c r="B217" s="43" t="str">
         <f t="shared" si="56"/>
@@ -14030,7 +14332,7 @@
       </c>
       <c r="AT218"/>
     </row>
-    <row r="219" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A219" s="36" t="s">
         <v>40</v>
       </c>
@@ -14086,7 +14388,7 @@
       <c r="AS219" s="17"/>
       <c r="AT219"/>
     </row>
-    <row r="220" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A220" s="36" t="s">
         <v>41</v>
       </c>
@@ -14138,7 +14440,7 @@
       <c r="AS220" s="17"/>
       <c r="AT220"/>
     </row>
-    <row r="221" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A221" s="36" t="s">
         <v>42</v>
       </c>
@@ -14190,7 +14492,7 @@
       <c r="AS221" s="17"/>
       <c r="AT221"/>
     </row>
-    <row r="222" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A222" s="36" t="s">
         <v>38</v>
       </c>
@@ -14250,7 +14552,7 @@
       </c>
       <c r="AS222" s="17"/>
     </row>
-    <row r="223" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A223" s="36" t="s">
         <v>145</v>
       </c>
@@ -14298,7 +14600,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="224" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A224" s="36" t="s">
         <v>143</v>
       </c>
@@ -14346,7 +14648,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="225" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A225" s="36" t="s">
         <v>429</v>
       </c>
@@ -14406,7 +14708,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="226" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A226" s="36" t="s">
         <v>124</v>
       </c>
@@ -14460,7 +14762,7 @@
       </c>
       <c r="AS226" s="17"/>
     </row>
-    <row r="227" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A227" s="36" t="s">
         <v>124</v>
       </c>
@@ -14508,7 +14810,7 @@
       </c>
       <c r="AS227" s="17"/>
     </row>
-    <row r="228" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A228" s="36" t="s">
         <v>128</v>
       </c>
@@ -14565,7 +14867,7 @@
       </c>
       <c r="AS228" s="33"/>
     </row>
-    <row r="229" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A229" s="36" t="s">
         <v>463</v>
       </c>
@@ -14613,7 +14915,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="230" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A230" s="36" t="s">
         <v>128</v>
       </c>
@@ -14661,7 +14963,7 @@
       </c>
       <c r="AS230" s="17"/>
     </row>
-    <row r="231" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A231" s="37" t="s">
         <v>181</v>
       </c>
@@ -14709,7 +15011,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="232" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A232" s="36" t="s">
         <v>130</v>
       </c>
@@ -14758,7 +15060,7 @@
       </c>
       <c r="AS232" s="17"/>
     </row>
-    <row r="233" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A233" s="36" t="s">
         <v>130</v>
       </c>
@@ -14804,7 +15106,7 @@
       </c>
       <c r="AS233" s="17"/>
     </row>
-    <row r="234" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A234" s="36" t="s">
         <v>163</v>
       </c>
@@ -14855,7 +15157,7 @@
       </c>
       <c r="AS234" s="17"/>
     </row>
-    <row r="235" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A235" s="36" t="s">
         <v>43</v>
       </c>
@@ -14909,7 +15211,7 @@
       </c>
       <c r="AS235" s="17"/>
     </row>
-    <row r="236" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A236" s="36" t="s">
         <v>44</v>
       </c>
@@ -14963,7 +15265,7 @@
       </c>
       <c r="AS236" s="17"/>
     </row>
-    <row r="237" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A237" s="36" t="s">
         <v>48</v>
       </c>
@@ -15011,7 +15313,7 @@
       </c>
       <c r="AS237" s="17"/>
     </row>
-    <row r="238" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A238" s="36" t="s">
         <v>90</v>
       </c>
@@ -15056,7 +15358,7 @@
       </c>
       <c r="AS238" s="17"/>
     </row>
-    <row r="239" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A239" s="37" t="s">
         <v>325</v>
       </c>
@@ -15104,7 +15406,7 @@
       </c>
       <c r="AS239" s="17"/>
     </row>
-    <row r="240" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A240" s="36" t="s">
         <v>133</v>
       </c>
@@ -15155,7 +15457,7 @@
       </c>
       <c r="AS240" s="33"/>
     </row>
-    <row r="241" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A241" s="36" t="s">
         <v>283</v>
       </c>
@@ -15203,7 +15505,7 @@
       </c>
       <c r="AS241" s="33"/>
     </row>
-    <row r="242" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A242" s="36" t="s">
         <v>142</v>
       </c>
@@ -15251,7 +15553,7 @@
       </c>
       <c r="AS242" s="33"/>
     </row>
-    <row r="243" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A243" s="36" t="s">
         <v>72</v>
       </c>
@@ -15296,7 +15598,7 @@
       </c>
       <c r="AS243" s="17"/>
     </row>
-    <row r="244" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A244" s="36" t="s">
         <v>73</v>
       </c>
@@ -15341,7 +15643,7 @@
       </c>
       <c r="AS244" s="17"/>
     </row>
-    <row r="245" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A245" s="36" t="s">
         <v>71</v>
       </c>
@@ -15386,7 +15688,7 @@
       </c>
       <c r="AS245" s="17"/>
     </row>
-    <row r="246" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A246" s="36" t="s">
         <v>76</v>
       </c>
@@ -15431,7 +15733,7 @@
       </c>
       <c r="AS246" s="17"/>
     </row>
-    <row r="247" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A247" s="36" t="s">
         <v>551</v>
       </c>
@@ -15476,7 +15778,7 @@
       </c>
       <c r="AS247" s="17"/>
     </row>
-    <row r="248" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A248" s="36" t="s">
         <v>273</v>
       </c>
@@ -15524,7 +15826,7 @@
       </c>
       <c r="AS248" s="51"/>
     </row>
-    <row r="249" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A249" s="36" t="s">
         <v>547</v>
       </c>
@@ -15569,7 +15871,7 @@
       </c>
       <c r="AS249" s="51"/>
     </row>
-    <row r="250" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A250" s="36" t="s">
         <v>548</v>
       </c>
@@ -15614,7 +15916,7 @@
       </c>
       <c r="AS250" s="51"/>
     </row>
-    <row r="251" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A251" s="36" t="s">
         <v>273</v>
       </c>
@@ -15659,7 +15961,7 @@
       </c>
       <c r="AS251" s="33"/>
     </row>
-    <row r="252" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A252" s="36" t="s">
         <v>216</v>
       </c>
@@ -15704,7 +16006,7 @@
       </c>
       <c r="AS252" s="17"/>
     </row>
-    <row r="253" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A253" s="36" t="s">
         <v>281</v>
       </c>
@@ -15749,7 +16051,7 @@
       </c>
       <c r="AS253" s="17"/>
     </row>
-    <row r="254" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A254" s="36" t="s">
         <v>549</v>
       </c>
@@ -15794,7 +16096,7 @@
       </c>
       <c r="AS254" s="24"/>
     </row>
-    <row r="255" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A255" s="36" t="s">
         <v>217</v>
       </c>
@@ -15839,7 +16141,7 @@
       </c>
       <c r="AS255" s="24"/>
     </row>
-    <row r="256" spans="1:45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A256" s="37" t="s">
         <v>114</v>
       </c>
@@ -15884,7 +16186,7 @@
       </c>
       <c r="AS256" s="24"/>
     </row>
-    <row r="257" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A257" s="36" t="s">
         <v>550</v>
       </c>
@@ -15929,7 +16231,7 @@
       </c>
       <c r="AS257" s="23"/>
     </row>
-    <row r="258" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A258" s="36" t="s">
         <v>74</v>
       </c>
@@ -15974,7 +16276,7 @@
       </c>
       <c r="AS258" s="23"/>
     </row>
-    <row r="259" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A259" s="36" t="s">
         <v>75</v>
       </c>
@@ -16019,7 +16321,7 @@
       </c>
       <c r="AS259" s="17"/>
     </row>
-    <row r="260" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A260" s="36" t="s">
         <v>274</v>
       </c>
@@ -16064,7 +16366,7 @@
       </c>
       <c r="AS260" s="17"/>
     </row>
-    <row r="261" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A261" s="36" t="s">
         <v>132</v>
       </c>
@@ -16115,7 +16417,7 @@
       </c>
       <c r="AS261" s="17"/>
     </row>
-    <row r="262" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A262" s="36" t="s">
         <v>132</v>
       </c>
@@ -16160,7 +16462,7 @@
       </c>
       <c r="AS262" s="17"/>
     </row>
-    <row r="263" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A263" s="36" t="s">
         <v>275</v>
       </c>
@@ -16205,7 +16507,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="264" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A264" s="36" t="s">
         <v>218</v>
       </c>
@@ -16250,7 +16552,7 @@
       </c>
       <c r="AS264" s="17"/>
     </row>
-    <row r="265" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A265" s="37" t="s">
         <v>115</v>
       </c>
@@ -16295,7 +16597,7 @@
       </c>
       <c r="AS265" s="17"/>
     </row>
-    <row r="266" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A266" s="36" t="s">
         <v>134</v>
       </c>
@@ -16340,7 +16642,7 @@
       </c>
       <c r="AS266" s="17"/>
     </row>
-    <row r="267" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A267" s="36" t="s">
         <v>83</v>
       </c>
@@ -16388,7 +16690,7 @@
       </c>
       <c r="AS267" s="29"/>
     </row>
-    <row r="268" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A268" s="36" t="s">
         <v>83</v>
       </c>
@@ -16421,7 +16723,7 @@
       <c r="AL268" s="35"/>
       <c r="AS268" s="45"/>
     </row>
-    <row r="269" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A269" s="36" t="s">
         <v>83</v>
       </c>
@@ -16484,7 +16786,7 @@
       </c>
       <c r="AS269" s="17"/>
     </row>
-    <row r="270" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A270" s="36" t="s">
         <v>334</v>
       </c>
@@ -16529,7 +16831,7 @@
       </c>
       <c r="AS270" s="33"/>
     </row>
-    <row r="271" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A271" s="36" t="s">
         <v>335</v>
       </c>
@@ -16574,7 +16876,7 @@
       </c>
       <c r="AS271" s="33"/>
     </row>
-    <row r="272" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A272" s="36" t="s">
         <v>336</v>
       </c>
@@ -16619,7 +16921,7 @@
       </c>
       <c r="AS272" s="33"/>
     </row>
-    <row r="273" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A273" s="36" t="s">
         <v>337</v>
       </c>
@@ -16664,7 +16966,7 @@
       </c>
       <c r="AS273" s="33"/>
     </row>
-    <row r="274" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:46" collapsed="1" x14ac:dyDescent="0.25">
       <c r="B274" s="43" t="str">
         <f t="shared" si="56"/>
         <v/>
@@ -16813,7 +17115,7 @@
       </c>
       <c r="AT275"/>
     </row>
-    <row r="276" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A276" s="36" t="s">
         <v>78</v>
       </c>
@@ -16859,7 +17161,7 @@
       <c r="AS276" s="17"/>
       <c r="AT276"/>
     </row>
-    <row r="277" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A277" s="36" t="s">
         <v>80</v>
       </c>
@@ -16905,7 +17207,7 @@
       <c r="AS277" s="17"/>
       <c r="AT277"/>
     </row>
-    <row r="278" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A278" s="36" t="s">
         <v>553</v>
       </c>
@@ -16951,7 +17253,7 @@
       <c r="AS278" s="17"/>
       <c r="AT278"/>
     </row>
-    <row r="279" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A279" s="36" t="s">
         <v>554</v>
       </c>
@@ -16997,7 +17299,7 @@
       <c r="AS279" s="17"/>
       <c r="AT279"/>
     </row>
-    <row r="280" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A280" s="36" t="s">
         <v>555</v>
       </c>
@@ -17043,7 +17345,7 @@
       <c r="AS280" s="17"/>
       <c r="AT280"/>
     </row>
-    <row r="281" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A281" s="36" t="s">
         <v>79</v>
       </c>
@@ -17089,7 +17391,7 @@
       <c r="AS281" s="17"/>
       <c r="AT281"/>
     </row>
-    <row r="282" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:46" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A282" s="16"/>
       <c r="B282" s="43" t="str">
         <f t="shared" si="66"/>
@@ -17264,7 +17566,7 @@
       </c>
       <c r="AT283"/>
     </row>
-    <row r="284" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A284" s="36" t="s">
         <v>396</v>
       </c>
@@ -17310,7 +17612,7 @@
       <c r="AS284" s="33"/>
       <c r="AT284"/>
     </row>
-    <row r="285" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A285" s="36" t="s">
         <v>93</v>
       </c>
@@ -17359,7 +17661,7 @@
       <c r="AS285" s="33"/>
       <c r="AT285"/>
     </row>
-    <row r="286" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A286" s="36" t="s">
         <v>188</v>
       </c>
@@ -17404,7 +17706,7 @@
       </c>
       <c r="AS286" s="33"/>
     </row>
-    <row r="287" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A287" s="36" t="s">
         <v>186</v>
       </c>
@@ -17449,7 +17751,7 @@
       </c>
       <c r="AS287" s="33"/>
     </row>
-    <row r="288" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A288" s="36" t="s">
         <v>185</v>
       </c>
@@ -17494,7 +17796,7 @@
       </c>
       <c r="AS288" s="33"/>
     </row>
-    <row r="289" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A289" s="36" t="s">
         <v>187</v>
       </c>
@@ -17539,7 +17841,7 @@
       </c>
       <c r="AS289" s="17"/>
     </row>
-    <row r="290" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A290" s="36" t="s">
         <v>522</v>
       </c>
@@ -17584,7 +17886,7 @@
       </c>
       <c r="AS290" s="34"/>
     </row>
-    <row r="291" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A291" s="36" t="s">
         <v>523</v>
       </c>
@@ -17629,7 +17931,7 @@
       </c>
       <c r="AS291" s="34"/>
     </row>
-    <row r="292" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A292" s="36" t="s">
         <v>503</v>
       </c>
@@ -17666,7 +17968,7 @@
       <c r="AS292" s="33"/>
       <c r="AT292"/>
     </row>
-    <row r="293" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A293" s="36" t="s">
         <v>500</v>
       </c>
@@ -17703,7 +18005,7 @@
       <c r="AS293" s="17"/>
       <c r="AT293"/>
     </row>
-    <row r="294" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A294" s="36" t="s">
         <v>502</v>
       </c>
@@ -17743,7 +18045,7 @@
       <c r="AS294" s="17"/>
       <c r="AT294"/>
     </row>
-    <row r="295" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A295" s="36" t="s">
         <v>514</v>
       </c>
@@ -17780,7 +18082,7 @@
       <c r="AS295" s="34"/>
       <c r="AT295"/>
     </row>
-    <row r="296" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A296" s="36" t="s">
         <v>244</v>
       </c>
@@ -17828,7 +18130,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="297" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A297" s="36" t="s">
         <v>515</v>
       </c>
@@ -17868,7 +18170,7 @@
       <c r="AS297" s="17"/>
       <c r="AT297"/>
     </row>
-    <row r="298" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A298" s="36" t="s">
         <v>516</v>
       </c>
@@ -17908,7 +18210,7 @@
       <c r="AS298" s="17"/>
       <c r="AT298"/>
     </row>
-    <row r="299" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A299" s="36" t="s">
         <v>83</v>
       </c>
@@ -17953,7 +18255,7 @@
       </c>
       <c r="AS299" s="33"/>
     </row>
-    <row r="300" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A300" s="36" t="s">
         <v>184</v>
       </c>
@@ -17998,7 +18300,7 @@
       </c>
       <c r="AS300" s="17"/>
     </row>
-    <row r="301" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A301" s="36" t="s">
         <v>94</v>
       </c>
@@ -18046,7 +18348,7 @@
       </c>
       <c r="AS301" s="34"/>
     </row>
-    <row r="302" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A302" s="36"/>
       <c r="B302" s="43" t="str">
         <f t="shared" si="70"/>
@@ -18084,7 +18386,7 @@
       <c r="AS302" s="17"/>
       <c r="AT302"/>
     </row>
-    <row r="303" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:46" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A303" s="16"/>
       <c r="B303" s="43" t="str">
         <f t="shared" si="66"/>
@@ -18258,7 +18560,7 @@
       </c>
       <c r="AT304"/>
     </row>
-    <row r="305" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A305" s="36" t="s">
         <v>245</v>
       </c>
@@ -18300,7 +18602,7 @@
       </c>
       <c r="AS305" s="17"/>
     </row>
-    <row r="306" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A306" s="36" t="s">
         <v>458</v>
       </c>
@@ -18342,7 +18644,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="307" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A307" s="36" t="s">
         <v>459</v>
       </c>
@@ -18387,7 +18689,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="308" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A308" s="36" t="s">
         <v>362</v>
       </c>
@@ -18430,7 +18732,7 @@
       </c>
       <c r="AS308" s="33"/>
     </row>
-    <row r="309" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A309" s="36" t="s">
         <v>362</v>
       </c>
@@ -18473,7 +18775,7 @@
       </c>
       <c r="AS309" s="17"/>
     </row>
-    <row r="310" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A310" s="36" t="s">
         <v>81</v>
       </c>
@@ -18554,7 +18856,7 @@
       </c>
       <c r="AS310" s="33"/>
     </row>
-    <row r="311" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A311" s="36" t="s">
         <v>81</v>
       </c>
@@ -18597,7 +18899,7 @@
       </c>
       <c r="AS311" s="33"/>
     </row>
-    <row r="312" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A312" s="36" t="s">
         <v>81</v>
       </c>
@@ -18661,7 +18963,7 @@
       </c>
       <c r="AS312" s="17"/>
     </row>
-    <row r="313" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A313" s="36" t="s">
         <v>249</v>
       </c>
@@ -18706,7 +19008,7 @@
       </c>
       <c r="AS313" s="17"/>
     </row>
-    <row r="314" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A314" s="36" t="s">
         <v>330</v>
       </c>
@@ -18748,7 +19050,7 @@
       </c>
       <c r="AS314" s="33"/>
     </row>
-    <row r="315" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A315" s="36" t="s">
         <v>331</v>
       </c>
@@ -18790,7 +19092,7 @@
       </c>
       <c r="AS315" s="33"/>
     </row>
-    <row r="316" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A316" s="36" t="s">
         <v>332</v>
       </c>
@@ -18832,7 +19134,7 @@
       </c>
       <c r="AS316" s="33"/>
     </row>
-    <row r="317" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A317" s="36" t="s">
         <v>333</v>
       </c>
@@ -18874,7 +19176,7 @@
       </c>
       <c r="AS317" s="33"/>
     </row>
-    <row r="318" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:46" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A318" s="16"/>
       <c r="B318" s="43" t="str">
         <f t="shared" si="66"/>
@@ -19038,7 +19340,7 @@
       </c>
       <c r="AT319"/>
     </row>
-    <row r="320" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A320" s="36" t="s">
         <v>246</v>
       </c>
@@ -19083,7 +19385,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="321" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A321" s="36" t="s">
         <v>279</v>
       </c>
@@ -19125,7 +19427,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="322" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:46" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A322" s="16"/>
       <c r="B322" s="43" t="str">
         <f t="shared" si="66"/>
@@ -19289,7 +19591,7 @@
       </c>
       <c r="AT323"/>
     </row>
-    <row r="324" spans="1:46" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:46" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="L324" s="33"/>
       <c r="M324" s="43" t="str">
         <f t="shared" si="67"/>
@@ -19313,7 +19615,7 @@
       <c r="AS324" s="23"/>
       <c r="AT324"/>
     </row>
-    <row r="325" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:46" collapsed="1" x14ac:dyDescent="0.25">
       <c r="L325" s="32" t="s">
         <v>13</v>
       </c>
@@ -20337,4 +20639,1464 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I119"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G127" sqref="G127"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="77.42578125" style="55" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>556</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>559</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>562</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>572</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>651</v>
+      </c>
+      <c r="I1" s="56" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I2" s="55" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>474</v>
+      </c>
+      <c r="G5" t="s">
+        <v>563</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I5" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>557</v>
+      </c>
+      <c r="G7" t="s">
+        <v>632</v>
+      </c>
+      <c r="I7" s="55" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>560</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>561</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>344</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>564</v>
+      </c>
+      <c r="G13" t="s">
+        <v>563</v>
+      </c>
+      <c r="I13" s="55" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>565</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>347</v>
+      </c>
+      <c r="G18" t="s">
+        <v>563</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I18" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>348</v>
+      </c>
+      <c r="G19" t="s">
+        <v>563</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I19" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>350</v>
+      </c>
+      <c r="G20" t="s">
+        <v>563</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I20" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>567</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>632</v>
+      </c>
+      <c r="I21" s="55" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>351</v>
+      </c>
+      <c r="G22" t="s">
+        <v>563</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I22" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>569</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>571</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>352</v>
+      </c>
+      <c r="G25" t="s">
+        <v>563</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I25" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>573</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>632</v>
+      </c>
+      <c r="I26" s="55" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>353</v>
+      </c>
+      <c r="G27" t="s">
+        <v>563</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I27" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>316</v>
+      </c>
+      <c r="I28" s="55" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>354</v>
+      </c>
+      <c r="G29" t="s">
+        <v>563</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I29" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>574</v>
+      </c>
+      <c r="G30" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I30" s="55" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>355</v>
+      </c>
+      <c r="G31" t="s">
+        <v>563</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I31" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>356</v>
+      </c>
+      <c r="G32" t="s">
+        <v>563</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I32" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>213</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>575</v>
+      </c>
+      <c r="G34" t="s">
+        <v>563</v>
+      </c>
+      <c r="I34" s="55" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>577</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>578</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>504</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>579</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>558</v>
+      </c>
+      <c r="I38" s="55" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I39" s="55" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>359</v>
+      </c>
+      <c r="G40" t="s">
+        <v>563</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I40" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>580</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>219</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>581</v>
+      </c>
+      <c r="G45" t="s">
+        <v>563</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I45" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>582</v>
+      </c>
+      <c r="G46" t="s">
+        <v>563</v>
+      </c>
+      <c r="I46" s="55" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>583</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" t="s">
+        <v>632</v>
+      </c>
+      <c r="I47" s="55" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>585</v>
+      </c>
+      <c r="G48" t="s">
+        <v>639</v>
+      </c>
+      <c r="I48" s="55" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>586</v>
+      </c>
+      <c r="I49" s="55" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>362</v>
+      </c>
+      <c r="G50" t="s">
+        <v>563</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I50" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>588</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" t="s">
+        <v>632</v>
+      </c>
+      <c r="I51" s="55" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>589</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>590</v>
+      </c>
+      <c r="G53" t="s">
+        <v>563</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I53" s="55" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>592</v>
+      </c>
+      <c r="G54" t="s">
+        <v>563</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I54" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>43</v>
+      </c>
+      <c r="G55" t="s">
+        <v>563</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I55" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>594</v>
+      </c>
+      <c r="G56" t="s">
+        <v>563</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I56" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>368</v>
+      </c>
+      <c r="G57" t="s">
+        <v>563</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I57" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>595</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G58" t="s">
+        <v>563</v>
+      </c>
+      <c r="I58" s="55" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>597</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>598</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>599</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>92</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>600</v>
+      </c>
+      <c r="G63" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I63" s="55" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>601</v>
+      </c>
+      <c r="G64" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I64" s="55" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>602</v>
+      </c>
+      <c r="G65" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I65" s="55" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>603</v>
+      </c>
+      <c r="G66" t="s">
+        <v>563</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I66" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>604</v>
+      </c>
+      <c r="G67" t="s">
+        <v>563</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I67" s="55" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>370</v>
+      </c>
+      <c r="G68" t="s">
+        <v>563</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I68" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>605</v>
+      </c>
+      <c r="G69" t="s">
+        <v>563</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I69" s="55" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>371</v>
+      </c>
+      <c r="G70" t="s">
+        <v>563</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I70" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>606</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I71" s="55" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>375</v>
+      </c>
+      <c r="G72" t="s">
+        <v>563</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I72" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>607</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>608</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G74" t="s">
+        <v>639</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I74" s="55" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>36</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G75" t="s">
+        <v>632</v>
+      </c>
+      <c r="I75" s="55" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>376</v>
+      </c>
+      <c r="G76" t="s">
+        <v>563</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I76" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>610</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>174</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>611</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>31</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>612</v>
+      </c>
+      <c r="G81" t="s">
+        <v>563</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I81" s="55" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>614</v>
+      </c>
+      <c r="G82" t="s">
+        <v>563</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I82" s="55" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>613</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G83" t="s">
+        <v>563</v>
+      </c>
+      <c r="I83" s="55" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>615</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G84" t="s">
+        <v>632</v>
+      </c>
+      <c r="I84" s="55" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>146</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>377</v>
+      </c>
+      <c r="G86" t="s">
+        <v>563</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I86" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>81</v>
+      </c>
+      <c r="G87" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I87" s="55" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>378</v>
+      </c>
+      <c r="G88" t="s">
+        <v>563</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I88" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>379</v>
+      </c>
+      <c r="G89" t="s">
+        <v>563</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I89" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>616</v>
+      </c>
+      <c r="G91" t="s">
+        <v>639</v>
+      </c>
+      <c r="I91" s="55" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>380</v>
+      </c>
+      <c r="G92" t="s">
+        <v>563</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I92" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>618</v>
+      </c>
+      <c r="G93" t="s">
+        <v>563</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I93" s="55" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>137</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G94" t="s">
+        <v>563</v>
+      </c>
+      <c r="I94" s="55" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>381</v>
+      </c>
+      <c r="G95" t="s">
+        <v>563</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I95" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>382</v>
+      </c>
+      <c r="G96" t="s">
+        <v>563</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I96" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>621</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G97" t="s">
+        <v>639</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I97" s="55" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>383</v>
+      </c>
+      <c r="G98" t="s">
+        <v>563</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I98" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>622</v>
+      </c>
+      <c r="G99" t="s">
+        <v>563</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I99" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>387</v>
+      </c>
+      <c r="G100" t="s">
+        <v>563</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I100" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>95</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>623</v>
+      </c>
+      <c r="G102" t="s">
+        <v>563</v>
+      </c>
+      <c r="I102" s="55" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>624</v>
+      </c>
+      <c r="G103" t="s">
+        <v>563</v>
+      </c>
+      <c r="I103" s="55" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>35</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>388</v>
+      </c>
+      <c r="G105" t="s">
+        <v>563</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I105" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>389</v>
+      </c>
+      <c r="G106" t="s">
+        <v>563</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I106" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>390</v>
+      </c>
+      <c r="G107" t="s">
+        <v>563</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I107" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>212</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>625</v>
+      </c>
+      <c r="G109" t="s">
+        <v>563</v>
+      </c>
+      <c r="I109" s="55" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>627</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>83</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G111" t="s">
+        <v>632</v>
+      </c>
+      <c r="I111" s="55" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>628</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>629</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>505</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>304</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G115" t="s">
+        <v>558</v>
+      </c>
+      <c r="I115" s="55" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>630</v>
+      </c>
+      <c r="G116" t="s">
+        <v>563</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I116" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>631</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>51</v>
+      </c>
+      <c r="G118" t="s">
+        <v>563</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I118" s="55" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>51</v>
+      </c>
+      <c r="G119" t="s">
+        <v>563</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I119" s="55" t="s">
+        <v>652</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I119">
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>